<commit_message>
state y consultarReserva (sin terminar)
</commit_message>
<xml_diff>
--- a/Casos-de-uso.xlsx
+++ b/Casos-de-uso.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12435" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12195" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D26"/>
+  <oleSize ref="A1:D14"/>
 </workbook>
 </file>
 
@@ -686,7 +686,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cambio de configuracion hibernet, algunas modificaciones en los jsp, agregue la relacion uno a uno en los mapeos Cliente y Login. Ahora subo el script de la bd-sistema-gestion-hotelera
</commit_message>
<xml_diff>
--- a/Casos-de-uso.xlsx
+++ b/Casos-de-uso.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12195" windowHeight="4830"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13005" windowHeight="3615"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:D14"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:D10"/>
 </workbook>
 </file>
 
@@ -350,8 +350,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -506,7 +505,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,14 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
@@ -697,7 +695,7 @@
     <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -725,7 +723,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -739,7 +737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -753,7 +751,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -767,7 +765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -784,7 +782,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -798,7 +796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -815,7 +813,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -829,7 +827,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -846,7 +844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -863,7 +861,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -883,14 +881,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -898,7 +896,7 @@
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -912,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -926,7 +924,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -940,7 +938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -954,7 +952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -968,7 +966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -982,7 +980,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -996,7 +994,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1010,7 +1008,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1027,7 +1025,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1044,7 +1042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1058,7 +1056,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1086,7 +1084,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1100,7 +1098,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1114,7 +1112,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1128,7 +1126,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1142,7 +1140,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1165,21 +1163,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1193,7 +1191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1210,7 +1208,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1227,7 +1225,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1241,7 +1239,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1255,7 +1253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1269,7 +1267,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1289,21 +1287,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1334,7 +1332,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1348,7 +1346,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1362,7 +1360,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1376,7 +1374,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1390,7 +1388,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1404,7 +1402,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1418,7 +1416,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1446,7 +1444,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1460,7 +1458,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1474,7 +1472,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1488,7 +1486,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1502,7 +1500,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Consumo de cliente en el hotel, generacion del ticket y algunas pantallas, falta que la recepcionista pueda confirmar reservas
</commit_message>
<xml_diff>
--- a/Casos-de-uso.xlsx
+++ b/Casos-de-uso.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13005" windowHeight="3615"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17865" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:D10"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M42"/>
 </workbook>
 </file>
 
@@ -350,8 +350,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,13 +359,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -380,8 +400,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,6 +494,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -505,6 +529,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -680,14 +705,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
@@ -695,7 +720,7 @@
     <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +734,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -723,7 +748,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -737,7 +762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -751,7 +776,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -765,7 +790,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -782,7 +807,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -796,14 +821,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
@@ -813,21 +838,21 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -844,7 +869,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -861,7 +886,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -877,18 +902,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -896,7 +922,7 @@
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -924,7 +950,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -938,7 +964,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -952,35 +978,35 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -994,21 +1020,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1025,14 +1051,14 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
@@ -1042,7 +1068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1056,35 +1082,35 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1098,7 +1124,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1112,7 +1138,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1126,7 +1152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1140,7 +1166,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1163,21 +1189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1208,7 +1234,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1225,7 +1251,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1239,7 +1265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1253,7 +1279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1267,7 +1293,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1287,21 +1313,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1315,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1332,7 +1358,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1346,7 +1372,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1360,7 +1386,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1374,7 +1400,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1388,7 +1414,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1402,7 +1428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1416,7 +1442,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1430,7 +1456,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1444,7 +1470,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1458,7 +1484,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1472,7 +1498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1486,7 +1512,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1500,7 +1526,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
modificacion diagrama de clases global y reserva.
</commit_message>
<xml_diff>
--- a/Casos-de-uso.xlsx
+++ b/Casos-de-uso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17865" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="10485" windowHeight="5070" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M42"/>
+  <oleSize ref="A1:D15"/>
 </workbook>
 </file>
 
@@ -910,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1192,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,17 +1293,17 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>